<commit_message>
pierwszy program + CubeMX
</commit_message>
<xml_diff>
--- a/kosztorys.xlsx
+++ b/kosztorys.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="8232" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PCB" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="163">
   <si>
     <t>Typ</t>
   </si>
@@ -511,6 +511,9 @@
   </si>
   <si>
     <t>kupione w tme</t>
+  </si>
+  <si>
+    <t>TME</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,12 +616,6 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -636,7 +633,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -678,9 +675,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -694,10 +688,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -1052,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,34 +1640,34 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="31" t="s">
+    <row r="22" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="31">
-        <v>0</v>
-      </c>
-      <c r="F22" s="34">
+      <c r="E22" s="28">
+        <v>0</v>
+      </c>
+      <c r="F22" s="31">
         <v>3.93</v>
       </c>
-      <c r="G22" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="31">
+      <c r="G22" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="28">
         <f t="shared" ref="I22:I23" si="2">E22*G$60</f>
         <v>0</v>
       </c>
-      <c r="K22" s="31" t="s">
+      <c r="K22" s="28" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1959,83 +1949,83 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+    <row r="33" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="10">
         <v>2</v>
       </c>
-      <c r="F33" s="26">
+      <c r="F33" s="12">
         <v>1.88</v>
       </c>
-      <c r="G33" s="27">
+      <c r="G33" s="13">
         <f t="shared" si="1"/>
         <v>3.76</v>
       </c>
-      <c r="I33" s="25">
+      <c r="I33" s="10">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="K33" s="25" t="s">
+      <c r="K33" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="M33" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="M33" s="25" t="s">
+      <c r="N33" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="12">
+        <v>2.93</v>
+      </c>
+      <c r="G34" s="13">
+        <f t="shared" si="1"/>
+        <v>2.93</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="M34" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="N33" s="25" t="s">
+      <c r="N34" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="O33" s="25" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="25">
-        <v>1</v>
-      </c>
-      <c r="F34" s="26">
-        <v>2.93</v>
-      </c>
-      <c r="G34" s="27">
-        <f t="shared" si="1"/>
-        <v>2.93</v>
-      </c>
-      <c r="I34" s="25">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K34" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="M34" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="N34" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="O34" s="25" t="s">
+      <c r="O34" s="10" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2686,31 +2676,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="29" t="s">
+    <row r="57" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
         <v>120</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E57" s="29">
+      <c r="E57" s="26">
         <v>1</v>
       </c>
       <c r="F57" s="12">
         <v>20.58</v>
       </c>
-      <c r="G57" s="30">
+      <c r="G57" s="27">
         <f t="shared" si="1"/>
         <v>20.58</v>
       </c>
-      <c r="I57" s="29">
-        <v>5</v>
-      </c>
-      <c r="J57" s="29">
+      <c r="I57" s="26">
+        <v>5</v>
+      </c>
+      <c r="J57" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59">
+        <f>SUM(E2:E57)</f>
+        <v>178</v>
+      </c>
       <c r="F59" s="4" t="s">
         <v>112</v>
       </c>
@@ -2829,7 +2826,7 @@
       <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>105</v>
       </c>
       <c r="D2">
@@ -2877,10 +2874,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="25"/>
       <c r="E5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2894,67 +2891,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="35">
         <v>6</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="35">
         <v>10.23</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
         <v>61.38</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="35">
         <f t="shared" si="2"/>
         <v>306.90000000000003</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="35">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:10" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="35">
         <v>6</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="35">
         <v>10.84</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
         <v>65.039999999999992</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="35">
         <f t="shared" si="2"/>
         <v>325.19999999999993</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="35">
         <v>18</v>
       </c>
     </row>
@@ -2987,7 +2984,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="34" t="s">
         <v>144</v>
       </c>
       <c r="E10">
@@ -3163,32 +3160,32 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+    <row r="16" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D16" s="31">
-        <v>0</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="31">
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="28" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3221,40 +3218,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31" t="s">
+    <row r="18" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="31">
-        <v>0</v>
-      </c>
-      <c r="E18" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="31">
+      <c r="D18" s="28">
+        <v>0</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="28" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="28"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="28"/>
+      <c r="C20" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
@@ -3265,7 +3262,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C25" s="28"/>
+      <c r="C25" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>